<commit_message>
integreted new login snd register system
</commit_message>
<xml_diff>
--- a/public/salesReport/salesReport.xlsx
+++ b/public/salesReport/salesReport.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="32">
   <si>
     <t>Serial Number</t>
   </si>
@@ -58,16 +58,19 @@
     <t>cashOnDelevery</t>
   </si>
   <si>
+    <t>seeeet, malapuram, kerala, 334355</t>
+  </si>
+  <si>
+    <t>"65681c96d2abb5eeeb6edd80"</t>
+  </si>
+  <si>
+    <t>Lenovo IdeaPad 3 14ITL6</t>
+  </si>
+  <si>
+    <t>Pay on Delivery (Cash/Card).</t>
+  </si>
+  <si>
     <t>smstreet, malapuram, kerala, 334355</t>
-  </si>
-  <si>
-    <t>"65681c96d2abb5eeeb6edd80"</t>
-  </si>
-  <si>
-    <t>Lenovo IdeaPad 3 14ITL6</t>
-  </si>
-  <si>
-    <t>Pay on Delivery (Cash/Card).</t>
   </si>
   <si>
     <t>razorPay</t>
@@ -594,7 +597,7 @@
         <v>18</v>
       </c>
       <c r="J3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -626,7 +629,7 @@
         <v>18</v>
       </c>
       <c r="J4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -658,7 +661,7 @@
         <v>18</v>
       </c>
       <c r="J5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -690,7 +693,7 @@
         <v>18</v>
       </c>
       <c r="J6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -719,10 +722,10 @@
         <v>13</v>
       </c>
       <c r="I7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" t="s">
         <v>19</v>
-      </c>
-      <c r="J7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -739,7 +742,7 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -751,10 +754,10 @@
         <v>13</v>
       </c>
       <c r="I8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -771,7 +774,7 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -783,10 +786,10 @@
         <v>13</v>
       </c>
       <c r="I9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -803,7 +806,7 @@
         <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -818,7 +821,7 @@
         <v>18</v>
       </c>
       <c r="J10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -835,7 +838,7 @@
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F11">
         <v>3</v>
@@ -850,7 +853,7 @@
         <v>18</v>
       </c>
       <c r="J11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -858,13 +861,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1">
         <v>45273.30324512732</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
         <v>17</v>
@@ -882,7 +885,7 @@
         <v>18</v>
       </c>
       <c r="J12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -890,16 +893,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1">
         <v>45273.30324512732</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -914,7 +917,7 @@
         <v>18</v>
       </c>
       <c r="J13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -931,7 +934,7 @@
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -943,10 +946,10 @@
         <v>13</v>
       </c>
       <c r="I14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -963,7 +966,7 @@
         <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F15">
         <v>3</v>
@@ -978,7 +981,7 @@
         <v>18</v>
       </c>
       <c r="J15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1010,7 +1013,7 @@
         <v>18</v>
       </c>
       <c r="J16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1027,7 +1030,7 @@
         <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F17">
         <v>2</v>
@@ -1042,7 +1045,7 @@
         <v>18</v>
       </c>
       <c r="J17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1059,7 +1062,7 @@
         <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1074,7 +1077,7 @@
         <v>18</v>
       </c>
       <c r="J18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1082,13 +1085,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C19" s="1">
         <v>45281.18030799768</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E19" t="s">
         <v>17</v>
@@ -1103,10 +1106,10 @@
         <v>13</v>
       </c>
       <c r="I19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>